<commit_message>
feat: Atualiza dados do Excel e URL da API para produção
- Atualiza base_barcos_dummy.xlsx com novos dados de veleiros
- Atualiza API_DOCUMENTATION.md com URL de produção (https://onbordo.onrender.com/)
- Remove documentação interativa local (Swagger UI/ReDoc) da documentação
- Mantém todos os endpoints e funcionalidades de filtros
</commit_message>
<xml_diff>
--- a/base_barcos_dummy.xlsx
+++ b/base_barcos_dummy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mateuspestana/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.pestana\Documents\onbordo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D55548-E156-4D49-9FE9-D3DDBEE0B7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A378D42-3C83-4B56-991C-7D0A671754B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="760" windowWidth="30000" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="73">
   <si>
     <t>ID do Barco</t>
   </si>
@@ -236,13 +236,19 @@
   </si>
   <si>
     <t>Kia Kaha II</t>
+  </si>
+  <si>
+    <t>Capitão Cloroquina</t>
+  </si>
+  <si>
+    <t>Amor Lindo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,6 +258,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -294,11 +308,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -317,9 +332,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -357,9 +372,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -392,9 +407,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -427,9 +459,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -603,21 +652,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.5" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.5" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -643,7 +692,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -669,7 +718,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -695,7 +744,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -721,7 +770,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -747,7 +796,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -773,7 +822,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -799,7 +848,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -825,7 +874,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -851,7 +900,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -877,7 +926,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -903,7 +952,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -929,7 +978,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -955,7 +1004,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -981,7 +1030,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1007,7 +1056,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1033,7 +1082,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1059,7 +1108,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1085,7 +1134,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1111,7 +1160,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1137,7 +1186,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1163,7 +1212,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1189,7 +1238,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1215,7 +1264,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1241,7 +1290,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1267,7 +1316,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1293,7 +1342,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1319,7 +1368,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1345,7 +1394,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1371,7 +1420,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1397,7 +1446,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1423,7 +1472,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1449,7 +1498,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1474,6 +1523,61 @@
       <c r="H33" t="s">
         <v>46</v>
       </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>1234</v>
+      </c>
+      <c r="C34" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34">
+        <v>25</v>
+      </c>
+      <c r="F34">
+        <v>8</v>
+      </c>
+      <c r="G34">
+        <v>512</v>
+      </c>
+      <c r="H34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>4321</v>
+      </c>
+      <c r="C35" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35">
+        <v>15</v>
+      </c>
+      <c r="F35">
+        <v>3</v>
+      </c>
+      <c r="G35">
+        <v>100</v>
+      </c>
+      <c r="H35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H32" xr:uid="{00000000-0001-0000-0000-000000000000}">
@@ -1482,5 +1586,6 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>